<commit_message>
optim script, update data
</commit_message>
<xml_diff>
--- a/data/FactorioPageList.xlsx
+++ b/data/FactorioPageList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\FactorioBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67CBF54-CBA4-4697-AAAF-2D130B42E997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69054C7F-0BB9-4E9E-8AB3-EACEEE407DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28845" yWindow="105" windowWidth="21825" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3778,8 +3778,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F457"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A411" sqref="A411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9526,7 +9526,7 @@
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
+      <c r="A289" s="3" t="s">
         <v>166</v>
       </c>
       <c r="B289" s="1">

</xml_diff>